<commit_message>
updated: good enough but still to fix small bug
</commit_message>
<xml_diff>
--- a/uploads/tawtarngathi.xlsx
+++ b/uploads/tawtarngathi.xlsx
@@ -25,7 +25,7 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>12</t>
+    <t>1</t>
   </si>
   <si>
     <t/>
@@ -37,7 +37,7 @@
     <t>09123456</t>
   </si>
   <si>
-    <t>14</t>
+    <t>2</t>
   </si>
   <si>
     <t>Htet</t>
@@ -46,7 +46,7 @@
     <t>09654321</t>
   </si>
   <si>
-    <t>16</t>
+    <t>3</t>
   </si>
   <si>
     <t>Htet Aung</t>
@@ -116,7 +116,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="381000" cy="190500"/>
+    <xdr:ext cx="476250" cy="285750"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1">
@@ -155,7 +155,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="381000" cy="190500"/>
+    <xdr:ext cx="476250" cy="285750"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 2">
@@ -194,7 +194,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="381000" cy="190500"/>
+    <xdr:ext cx="476250" cy="285750"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 3">
@@ -554,7 +554,7 @@
   <dimension ref="A1:D4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -572,7 +572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" ht="40" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -586,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" ht="40" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -600,7 +600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" ht="40" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>

</xml_diff>